<commit_message>
RPA-114: Etter disksjon med Arild og Sissel i møte avklaring om aaintekt del 2
</commit_message>
<xml_diff>
--- a/Vasklister/prossesbeskrivelser/2016-12-14 VASKELISTER_DEL1_v2.1 KVS_dokument Godkjent.xlsx
+++ b/Vasklister/prossesbeskrivelser/2016-12-14 VASKELISTER_DEL1_v2.1 KVS_dokument Godkjent.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15456" windowHeight="9732" tabRatio="810"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15450" windowHeight="9735" tabRatio="810"/>
   </bookViews>
   <sheets>
     <sheet name="Prosessbeskrivelse" sheetId="1" r:id="rId1"/>
@@ -465,10 +465,6 @@
   </si>
   <si>
     <t>Gå til Total A-Inntekt (Ved arbeidsgiver)</t>
-  </si>
-  <si>
-    <t>Avgjør hva man gjør i DEL 2 av VL-prosess.
-Utbroder her senere.</t>
   </si>
   <si>
     <t>Gå til Økonomisk oppsett med skatt</t>
@@ -1412,6 +1408,9 @@
   </si>
   <si>
     <t>Regneark + skjermdump UB (Utleggsdatabasen)</t>
+  </si>
+  <si>
+    <t>Vi lagerer alle linjer ved treff i aaintekt.</t>
   </si>
 </sst>
 </file>
@@ -2199,6 +2198,9 @@
     <xf numFmtId="0" fontId="24" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2219,9 +2221,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -13777,7 +13776,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -13787,76 +13786,76 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="B184" sqref="B184"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.44140625" customWidth="1"/>
-    <col min="2" max="2" width="39.5546875" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.44140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.109375" customWidth="1"/>
-    <col min="6" max="6" width="31.5546875" customWidth="1"/>
-    <col min="7" max="7" width="41.88671875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.42578125" customWidth="1"/>
+    <col min="2" max="2" width="39.5703125" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.42578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.140625" customWidth="1"/>
+    <col min="6" max="6" width="31.5703125" customWidth="1"/>
+    <col min="7" max="7" width="41.85546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="38" style="2" customWidth="1"/>
-    <col min="11" max="11" width="42.33203125" customWidth="1"/>
+    <col min="11" max="11" width="42.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="34.5" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B2" s="147" t="s">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B2" s="148" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="149" t="s">
+      <c r="C2" s="150" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="149"/>
-      <c r="E2" s="149"/>
-      <c r="F2" s="149"/>
-      <c r="G2" s="149"/>
-      <c r="H2" s="149"/>
+      <c r="D2" s="150"/>
+      <c r="E2" s="150"/>
+      <c r="F2" s="150"/>
+      <c r="G2" s="150"/>
+      <c r="H2" s="150"/>
       <c r="I2" s="3"/>
       <c r="J2" s="63"/>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B3" s="148"/>
-      <c r="C3" s="149" t="s">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B3" s="149"/>
+      <c r="C3" s="150" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="149"/>
-      <c r="E3" s="149"/>
-      <c r="F3" s="149"/>
-      <c r="G3" s="149"/>
-      <c r="H3" s="149"/>
+      <c r="D3" s="150"/>
+      <c r="E3" s="150"/>
+      <c r="F3" s="150"/>
+      <c r="G3" s="150"/>
+      <c r="H3" s="150"/>
       <c r="I3" s="3"/>
       <c r="J3" s="63"/>
     </row>
-    <row r="4" spans="2:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="150" t="s">
-        <v>263</v>
-      </c>
-      <c r="D4" s="150"/>
-      <c r="E4" s="150"/>
-      <c r="F4" s="150"/>
-      <c r="G4" s="150"/>
-      <c r="H4" s="150"/>
+      <c r="C4" s="151" t="s">
+        <v>262</v>
+      </c>
+      <c r="D4" s="151"/>
+      <c r="E4" s="151"/>
+      <c r="F4" s="151"/>
+      <c r="G4" s="151"/>
+      <c r="H4" s="151"/>
       <c r="I4" s="5"/>
       <c r="J4" s="61"/>
     </row>
-    <row r="5" spans="2:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="5"/>
       <c r="C5" s="12"/>
       <c r="D5" s="17"/>
@@ -13867,7 +13866,7 @@
       <c r="I5" s="5"/>
       <c r="J5" s="61"/>
     </row>
-    <row r="6" spans="2:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
         <v>2</v>
       </c>
@@ -13879,7 +13878,7 @@
       </c>
       <c r="F6" s="9"/>
     </row>
-    <row r="7" spans="2:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="6"/>
       <c r="C7" s="7"/>
       <c r="D7" s="8"/>
@@ -13891,7 +13890,7 @@
       </c>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="64" t="s">
         <v>5</v>
       </c>
@@ -13922,7 +13921,7 @@
       <c r="K9" s="66"/>
       <c r="L9" s="66"/>
     </row>
-    <row r="10" spans="2:12" ht="24" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:12" ht="24" x14ac:dyDescent="0.25">
       <c r="B10" s="48" t="s">
         <v>17</v>
       </c>
@@ -13949,11 +13948,11 @@
       </c>
       <c r="J10" s="50"/>
       <c r="K10" s="54" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="L10" s="54"/>
     </row>
-    <row r="11" spans="2:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" s="52"/>
       <c r="C11" s="53"/>
       <c r="D11" s="54"/>
@@ -13966,7 +13965,7 @@
       <c r="K11" s="54"/>
       <c r="L11" s="54"/>
     </row>
-    <row r="12" spans="2:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" s="55"/>
       <c r="C12" s="53"/>
       <c r="D12" s="54"/>
@@ -13985,7 +13984,7 @@
       </c>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" s="64" t="s">
         <v>5</v>
       </c>
@@ -14016,7 +14015,7 @@
       <c r="K15" s="66"/>
       <c r="L15" s="66"/>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" s="29" t="s">
         <v>35</v>
       </c>
@@ -14024,7 +14023,7 @@
         <v>1</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E16" s="29"/>
       <c r="F16" s="41"/>
@@ -14037,17 +14036,17 @@
       <c r="K16" s="29"/>
       <c r="L16" s="29"/>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="42"/>
       <c r="C17" s="137" t="s">
+        <v>289</v>
+      </c>
+      <c r="D17" s="138" t="s">
         <v>290</v>
-      </c>
-      <c r="D17" s="138" t="s">
-        <v>291</v>
       </c>
       <c r="E17" s="29"/>
       <c r="F17" s="41" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G17" s="40"/>
       <c r="H17" s="41"/>
@@ -14056,13 +14055,13 @@
       <c r="K17" s="29"/>
       <c r="L17" s="29"/>
     </row>
-    <row r="18" spans="2:12" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="41"/>
       <c r="C18" s="30">
         <v>2</v>
       </c>
       <c r="D18" s="29" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E18" s="29"/>
       <c r="F18" s="40" t="s">
@@ -14075,7 +14074,7 @@
       <c r="K18" s="29"/>
       <c r="L18" s="29"/>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="42"/>
       <c r="C19" s="36">
         <v>3</v>
@@ -14092,11 +14091,11 @@
       <c r="I19" s="41"/>
       <c r="J19" s="40"/>
       <c r="K19" s="29" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L19" s="29"/>
     </row>
-    <row r="20" spans="2:12" ht="60" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:12" ht="60" x14ac:dyDescent="0.25">
       <c r="B20" s="29"/>
       <c r="C20" s="30">
         <v>4</v>
@@ -14117,11 +14116,11 @@
         <v>73</v>
       </c>
       <c r="K20" s="29" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L20" s="29"/>
     </row>
-    <row r="21" spans="2:12" ht="130.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:12" ht="130.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="19" t="s">
         <v>36</v>
       </c>
@@ -14136,19 +14135,19 @@
         <v>37</v>
       </c>
       <c r="G21" s="39" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H21" s="19"/>
       <c r="I21" s="19"/>
       <c r="J21" s="20"/>
       <c r="K21" s="20" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="L21" s="20" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12" ht="95.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" ht="95.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="32" t="s">
         <v>39</v>
       </c>
@@ -14163,17 +14162,17 @@
         <v>41</v>
       </c>
       <c r="G22" s="34" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H22" s="32"/>
       <c r="I22" s="32"/>
       <c r="J22" s="34"/>
       <c r="K22" s="34" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="L22" s="34"/>
     </row>
-    <row r="23" spans="2:12" ht="96" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:12" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="26" t="s">
         <v>40</v>
       </c>
@@ -14188,17 +14187,17 @@
         <v>44</v>
       </c>
       <c r="G23" s="141" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H23" s="26"/>
       <c r="I23" s="26"/>
       <c r="J23" s="141" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="K23" s="28"/>
       <c r="L23" s="28"/>
     </row>
-    <row r="24" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="21" t="s">
         <v>50</v>
       </c>
@@ -14210,18 +14209,18 @@
       </c>
       <c r="E24" s="21"/>
       <c r="F24" s="24"/>
-      <c r="G24" s="151" t="s">
+      <c r="G24" s="152" t="s">
         <v>78</v>
       </c>
       <c r="H24" s="21"/>
       <c r="I24" s="21"/>
       <c r="J24" s="24"/>
       <c r="K24" s="24" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L24" s="24"/>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" s="21"/>
       <c r="C25" s="22" t="s">
         <v>53</v>
@@ -14231,16 +14230,16 @@
       </c>
       <c r="E25" s="21"/>
       <c r="F25" s="24"/>
-      <c r="G25" s="152"/>
+      <c r="G25" s="153"/>
       <c r="H25" s="21"/>
       <c r="I25" s="21"/>
       <c r="J25" s="24"/>
       <c r="K25" s="24" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L25" s="24"/>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" s="21"/>
       <c r="C26" s="22" t="s">
         <v>54</v>
@@ -14250,16 +14249,16 @@
       </c>
       <c r="E26" s="21"/>
       <c r="F26" s="24"/>
-      <c r="G26" s="152"/>
+      <c r="G26" s="153"/>
       <c r="H26" s="21"/>
       <c r="I26" s="21"/>
       <c r="J26" s="24"/>
       <c r="K26" s="24" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L26" s="24"/>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" s="21"/>
       <c r="C27" s="22" t="s">
         <v>55</v>
@@ -14269,14 +14268,14 @@
       </c>
       <c r="E27" s="21"/>
       <c r="F27" s="24"/>
-      <c r="G27" s="152"/>
+      <c r="G27" s="153"/>
       <c r="H27" s="21"/>
       <c r="I27" s="21"/>
       <c r="J27" s="24"/>
       <c r="K27" s="24"/>
       <c r="L27" s="24"/>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B28" s="21"/>
       <c r="C28" s="22" t="s">
         <v>56</v>
@@ -14286,14 +14285,14 @@
       </c>
       <c r="E28" s="21"/>
       <c r="F28" s="24"/>
-      <c r="G28" s="152"/>
+      <c r="G28" s="153"/>
       <c r="H28" s="21"/>
       <c r="I28" s="21"/>
       <c r="J28" s="24"/>
       <c r="K28" s="24"/>
       <c r="L28" s="24"/>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B29" s="21"/>
       <c r="C29" s="22" t="s">
         <v>57</v>
@@ -14303,16 +14302,16 @@
       </c>
       <c r="E29" s="21"/>
       <c r="F29" s="24"/>
-      <c r="G29" s="152"/>
+      <c r="G29" s="153"/>
       <c r="H29" s="21"/>
       <c r="I29" s="21"/>
       <c r="J29" s="24"/>
       <c r="K29" s="24" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L29" s="24"/>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B30" s="21"/>
       <c r="C30" s="22" t="s">
         <v>58</v>
@@ -14324,16 +14323,16 @@
         <v>51</v>
       </c>
       <c r="F30" s="24"/>
-      <c r="G30" s="152"/>
+      <c r="G30" s="153"/>
       <c r="H30" s="21"/>
       <c r="I30" s="21"/>
       <c r="J30" s="24"/>
       <c r="K30" s="24" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="L30" s="24"/>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B31" s="21"/>
       <c r="C31" s="22" t="s">
         <v>60</v>
@@ -14345,16 +14344,16 @@
         <v>61</v>
       </c>
       <c r="F31" s="24"/>
-      <c r="G31" s="152"/>
+      <c r="G31" s="153"/>
       <c r="H31" s="21"/>
       <c r="I31" s="21"/>
       <c r="J31" s="24"/>
       <c r="K31" s="24" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="L31" s="24"/>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B32" s="21"/>
       <c r="C32" s="22" t="s">
         <v>75</v>
@@ -14364,20 +14363,20 @@
       </c>
       <c r="E32" s="21"/>
       <c r="F32" s="24"/>
-      <c r="G32" s="153"/>
+      <c r="G32" s="154"/>
       <c r="H32" s="21"/>
       <c r="I32" s="21"/>
       <c r="J32" s="24"/>
       <c r="K32" s="24"/>
       <c r="L32" s="24"/>
     </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B33" s="21"/>
       <c r="C33" s="140" t="s">
+        <v>294</v>
+      </c>
+      <c r="D33" s="139" t="s">
         <v>295</v>
-      </c>
-      <c r="D33" s="139" t="s">
-        <v>296</v>
       </c>
       <c r="E33" s="21"/>
       <c r="F33" s="24"/>
@@ -14388,9 +14387,9 @@
       <c r="K33" s="24"/>
       <c r="L33" s="24"/>
     </row>
-    <row r="34" spans="2:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="29" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C34" s="36">
         <v>8</v>
@@ -14402,20 +14401,20 @@
         <v>63</v>
       </c>
       <c r="F34" s="37" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G34" s="37" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H34" s="29"/>
       <c r="I34" s="29"/>
       <c r="J34" s="31" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="K34" s="31"/>
       <c r="L34" s="31"/>
     </row>
-    <row r="35" spans="2:12" ht="38.4" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:12" ht="39" x14ac:dyDescent="0.25">
       <c r="B35" s="29" t="s">
         <v>66</v>
       </c>
@@ -14432,17 +14431,17 @@
         <v>67</v>
       </c>
       <c r="G35" s="37" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="H35" s="29"/>
       <c r="I35" s="29"/>
       <c r="J35" s="31"/>
       <c r="K35" s="31" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L35" s="31"/>
     </row>
-    <row r="36" spans="2:12" ht="36" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:12" ht="36" x14ac:dyDescent="0.25">
       <c r="B36" s="29" t="s">
         <v>66</v>
       </c>
@@ -14461,13 +14460,13 @@
       <c r="I36" s="29"/>
       <c r="J36" s="31"/>
       <c r="K36" s="31" t="s">
+        <v>211</v>
+      </c>
+      <c r="L36" s="31" t="s">
         <v>212</v>
       </c>
-      <c r="L36" s="31" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B37" s="58"/>
       <c r="C37" s="59">
         <v>11</v>
@@ -14486,7 +14485,7 @@
       <c r="K37" s="60"/>
       <c r="L37" s="60"/>
     </row>
-    <row r="38" spans="2:12" ht="108.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:12" ht="108.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="58"/>
       <c r="C38" s="59">
         <v>12</v>
@@ -14503,11 +14502,11 @@
         <v>72</v>
       </c>
       <c r="K38" s="60" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="L38" s="60"/>
     </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="K39" s="102"/>
       <c r="L39" s="103"/>
     </row>
@@ -14517,7 +14516,7 @@
       </c>
       <c r="F40" s="2"/>
     </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B41" s="64" t="s">
         <v>5</v>
       </c>
@@ -14548,7 +14547,7 @@
       <c r="K41" s="66"/>
       <c r="L41" s="66"/>
     </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B42" s="97" t="s">
         <v>80</v>
       </c>
@@ -14567,7 +14566,7 @@
       <c r="K42" s="99"/>
       <c r="L42" s="99"/>
     </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B43" s="97"/>
       <c r="C43" s="38">
         <v>2</v>
@@ -14586,7 +14585,7 @@
       <c r="K43" s="99"/>
       <c r="L43" s="99"/>
     </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B44" s="97"/>
       <c r="C44" s="38">
         <v>3</v>
@@ -14595,7 +14594,7 @@
         <v>49</v>
       </c>
       <c r="E44" s="99" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F44" s="99"/>
       <c r="G44" s="99"/>
@@ -14605,7 +14604,7 @@
       <c r="K44" s="99"/>
       <c r="L44" s="99"/>
     </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B45" s="97"/>
       <c r="C45" s="38">
         <v>4</v>
@@ -14622,7 +14621,7 @@
       <c r="K45" s="99"/>
       <c r="L45" s="99"/>
     </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B46" s="97"/>
       <c r="C46" s="38">
         <v>5</v>
@@ -14637,7 +14636,7 @@
       <c r="K46" s="99"/>
       <c r="L46" s="99"/>
     </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B47" s="97"/>
       <c r="C47" s="38">
         <v>6</v>
@@ -14658,7 +14657,7 @@
       </c>
       <c r="F49" s="2"/>
     </row>
-    <row r="50" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B50" s="64" t="s">
         <v>5</v>
       </c>
@@ -14689,7 +14688,7 @@
       <c r="K50" s="66"/>
       <c r="L50" s="66"/>
     </row>
-    <row r="51" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B51" s="80"/>
       <c r="C51" s="27">
         <v>1</v>
@@ -14710,7 +14709,7 @@
       <c r="K51" s="81"/>
       <c r="L51" s="81"/>
     </row>
-    <row r="52" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B52" s="80"/>
       <c r="C52" s="27">
         <v>2</v>
@@ -14725,11 +14724,11 @@
       <c r="I52" s="80"/>
       <c r="J52" s="81"/>
       <c r="K52" s="81" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="L52" s="81"/>
     </row>
-    <row r="53" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B53" s="80"/>
       <c r="C53" s="27">
         <v>3</v>
@@ -14746,7 +14745,7 @@
       <c r="K53" s="81"/>
       <c r="L53" s="81"/>
     </row>
-    <row r="54" spans="2:12" ht="24" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:12" ht="24" x14ac:dyDescent="0.25">
       <c r="B54" s="80"/>
       <c r="C54" s="27">
         <v>4</v>
@@ -14767,7 +14766,7 @@
       <c r="K54" s="81"/>
       <c r="L54" s="81"/>
     </row>
-    <row r="55" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B55" s="80"/>
       <c r="C55" s="27">
         <v>5</v>
@@ -14786,7 +14785,7 @@
       <c r="K55" s="81"/>
       <c r="L55" s="81"/>
     </row>
-    <row r="56" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B56" s="80"/>
       <c r="C56" s="27">
         <v>6</v>
@@ -14803,7 +14802,7 @@
       <c r="K56" s="81"/>
       <c r="L56" s="81"/>
     </row>
-    <row r="57" spans="2:12" ht="48.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:12" ht="48.75" x14ac:dyDescent="0.25">
       <c r="B57" s="80"/>
       <c r="C57" s="27">
         <v>7</v>
@@ -14816,17 +14815,17 @@
       </c>
       <c r="F57" s="80"/>
       <c r="G57" s="143" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H57" s="80"/>
       <c r="I57" s="80"/>
       <c r="J57" s="81"/>
       <c r="K57" s="81" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="L57" s="81"/>
     </row>
-    <row r="58" spans="2:12" ht="24" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B58" s="80"/>
       <c r="C58" s="27">
         <v>8</v>
@@ -14842,16 +14841,16 @@
       <c r="H58" s="80"/>
       <c r="I58" s="80"/>
       <c r="J58" s="104" t="s">
-        <v>99</v>
+        <v>308</v>
       </c>
       <c r="K58" s="81" t="s">
+        <v>216</v>
+      </c>
+      <c r="L58" s="81" t="s">
         <v>217</v>
       </c>
-      <c r="L58" s="81" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="59" spans="2:12" ht="24" x14ac:dyDescent="0.3">
+    </row>
+    <row r="59" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B59" s="80"/>
       <c r="C59" s="27">
         <v>9</v>
@@ -14867,20 +14866,20 @@
       <c r="H59" s="80"/>
       <c r="I59" s="80"/>
       <c r="J59" s="104" t="s">
-        <v>99</v>
+        <v>308</v>
       </c>
       <c r="K59" s="81" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L59" s="81"/>
     </row>
-    <row r="60" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B60" s="80"/>
       <c r="C60" s="27">
         <v>10</v>
       </c>
       <c r="D60" s="80" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E60" s="80"/>
       <c r="F60" s="80"/>
@@ -14890,16 +14889,16 @@
       <c r="J60" s="81"/>
       <c r="K60" s="81"/>
       <c r="L60" s="81" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="62" spans="2:12" ht="18" x14ac:dyDescent="0.35">
       <c r="B62" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F62" s="2"/>
     </row>
-    <row r="63" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B63" s="64" t="s">
         <v>5</v>
       </c>
@@ -14930,13 +14929,13 @@
       <c r="K63" s="66"/>
       <c r="L63" s="66"/>
     </row>
-    <row r="64" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B64" s="95"/>
       <c r="C64" s="56">
         <v>1</v>
       </c>
       <c r="D64" s="95" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E64" s="96"/>
       <c r="F64" s="95"/>
@@ -14945,20 +14944,20 @@
       <c r="I64" s="95"/>
       <c r="J64" s="96"/>
       <c r="K64" s="96" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="L64" s="96"/>
     </row>
-    <row r="65" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:14" ht="24" x14ac:dyDescent="0.25">
       <c r="B65" s="95"/>
       <c r="C65" s="56">
         <v>2</v>
       </c>
       <c r="D65" s="95" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E65" s="96" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F65" s="95"/>
       <c r="G65" s="96"/>
@@ -14966,20 +14965,20 @@
       <c r="I65" s="95"/>
       <c r="J65" s="96"/>
       <c r="K65" s="96" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="L65" s="96"/>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B66" s="95"/>
       <c r="C66" s="56">
         <v>3</v>
       </c>
       <c r="D66" s="95" t="s">
+        <v>133</v>
+      </c>
+      <c r="E66" s="96" t="s">
         <v>134</v>
-      </c>
-      <c r="E66" s="96" t="s">
-        <v>135</v>
       </c>
       <c r="F66" s="95"/>
       <c r="G66" s="96"/>
@@ -14987,20 +14986,20 @@
       <c r="I66" s="95"/>
       <c r="J66" s="96"/>
       <c r="K66" s="96" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L66" s="96"/>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B67" s="95"/>
       <c r="C67" s="56">
         <v>4</v>
       </c>
       <c r="D67" s="144" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E67" s="96" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F67" s="95"/>
       <c r="G67" s="96"/>
@@ -15008,17 +15007,17 @@
       <c r="I67" s="95"/>
       <c r="J67" s="96"/>
       <c r="K67" s="96" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="L67" s="96"/>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B68" s="95"/>
       <c r="C68" s="56">
         <v>5</v>
       </c>
       <c r="D68" s="95" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E68" s="96"/>
       <c r="F68" s="95"/>
@@ -15027,23 +15026,23 @@
       <c r="I68" s="95"/>
       <c r="J68" s="96"/>
       <c r="K68" s="96" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="L68" s="96"/>
     </row>
-    <row r="70" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A70" s="135" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B70" s="10" t="s">
+        <v>286</v>
+      </c>
+      <c r="D70" s="132" t="s">
         <v>287</v>
       </c>
-      <c r="D70" s="132" t="s">
-        <v>288</v>
-      </c>
       <c r="F70" s="2"/>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B71" s="64" t="s">
         <v>5</v>
       </c>
@@ -15074,13 +15073,13 @@
       <c r="K71" s="68"/>
       <c r="L71" s="68"/>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B72" s="94"/>
       <c r="C72" s="94">
         <v>1</v>
       </c>
       <c r="D72" s="94" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E72" s="94"/>
       <c r="F72" s="94"/>
@@ -15092,13 +15091,13 @@
       <c r="L72" s="94"/>
       <c r="N72" s="114"/>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B73" s="94"/>
       <c r="C73" s="94">
         <v>2</v>
       </c>
       <c r="D73" s="94" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E73" s="94"/>
       <c r="F73" s="94"/>
@@ -15110,7 +15109,7 @@
       <c r="L73" s="94"/>
       <c r="N73" s="114"/>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B74" s="94"/>
       <c r="C74" s="94"/>
       <c r="D74" s="94"/>
@@ -15124,13 +15123,13 @@
       <c r="L74" s="94"/>
       <c r="N74" s="115"/>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B75" s="94"/>
       <c r="C75" s="94">
         <v>4</v>
       </c>
       <c r="D75" s="94" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E75" s="94"/>
       <c r="F75" s="94"/>
@@ -15142,13 +15141,13 @@
       <c r="L75" s="94"/>
       <c r="N75" s="115"/>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B76" s="94"/>
       <c r="C76" s="94">
         <v>5</v>
       </c>
       <c r="D76" s="94" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E76" s="94"/>
       <c r="F76" s="94"/>
@@ -15160,13 +15159,13 @@
       <c r="L76" s="94"/>
       <c r="N76" s="115"/>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B77" s="94"/>
       <c r="C77" s="94">
         <v>6</v>
       </c>
       <c r="D77" s="94" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E77" s="94"/>
       <c r="F77" s="94"/>
@@ -15178,13 +15177,13 @@
       <c r="L77" s="94"/>
       <c r="N77" s="115"/>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B78" s="94"/>
       <c r="C78" s="94">
         <v>7</v>
       </c>
       <c r="D78" s="94" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E78" s="94"/>
       <c r="F78" s="94"/>
@@ -15196,28 +15195,28 @@
       <c r="L78" s="94"/>
       <c r="N78" s="115"/>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="D79" s="115"/>
       <c r="N79" s="115"/>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="D80" s="115"/>
       <c r="N80" s="115"/>
     </row>
-    <row r="81" spans="1:12" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A81" s="135" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B81" s="10" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C81" s="116"/>
       <c r="D81" s="132" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F81" s="2"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B82" s="64" t="s">
         <v>5</v>
       </c>
@@ -15248,16 +15247,16 @@
       <c r="K82" s="68"/>
       <c r="L82" s="68"/>
     </row>
-    <row r="83" spans="1:12" ht="24" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:12" ht="24" x14ac:dyDescent="0.25">
       <c r="B83" s="117"/>
       <c r="C83" s="118">
         <v>1</v>
       </c>
       <c r="D83" s="134" t="s">
+        <v>136</v>
+      </c>
+      <c r="E83" s="133" t="s">
         <v>137</v>
-      </c>
-      <c r="E83" s="133" t="s">
-        <v>138</v>
       </c>
       <c r="F83" s="117"/>
       <c r="G83" s="133"/>
@@ -15265,47 +15264,47 @@
       <c r="I83" s="134"/>
       <c r="J83" s="133"/>
       <c r="K83" s="133" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="L83" s="119"/>
     </row>
-    <row r="84" spans="1:12" ht="48" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:12" ht="48" x14ac:dyDescent="0.25">
       <c r="B84" s="117"/>
       <c r="C84" s="118">
         <v>2</v>
       </c>
       <c r="D84" s="145" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E84" s="133" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F84" s="117"/>
       <c r="G84" s="133" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="H84" s="134"/>
       <c r="I84" s="134"/>
       <c r="J84" s="133"/>
       <c r="K84" s="133" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L84" s="119"/>
     </row>
-    <row r="85" spans="1:12" ht="24" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:12" ht="24" x14ac:dyDescent="0.25">
       <c r="B85" s="117"/>
       <c r="C85" s="118">
         <v>3</v>
       </c>
       <c r="D85" s="134" t="s">
+        <v>139</v>
+      </c>
+      <c r="E85" s="133" t="s">
         <v>140</v>
-      </c>
-      <c r="E85" s="133" t="s">
-        <v>141</v>
       </c>
       <c r="F85" s="117"/>
       <c r="G85" s="133" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H85" s="134"/>
       <c r="I85" s="134"/>
@@ -15313,14 +15312,14 @@
       <c r="K85" s="133"/>
       <c r="L85" s="119"/>
     </row>
-    <row r="86" spans="1:12" ht="24" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:12" ht="24" x14ac:dyDescent="0.25">
       <c r="B86" s="117"/>
       <c r="C86" s="118">
         <v>4</v>
       </c>
       <c r="D86" s="134"/>
       <c r="E86" s="133" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F86" s="117"/>
       <c r="G86" s="133"/>
@@ -15328,18 +15327,18 @@
       <c r="I86" s="134"/>
       <c r="J86" s="133"/>
       <c r="K86" s="133" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="L86" s="119"/>
     </row>
-    <row r="87" spans="1:12" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:12" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B87" s="117"/>
       <c r="C87" s="118">
         <v>5</v>
       </c>
       <c r="D87" s="134"/>
       <c r="E87" s="133" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F87" s="117"/>
       <c r="G87" s="133"/>
@@ -15349,13 +15348,13 @@
       <c r="K87" s="133"/>
       <c r="L87" s="119"/>
     </row>
-    <row r="88" spans="1:12" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:12" ht="20.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B88" s="117"/>
       <c r="C88" s="118">
         <v>6</v>
       </c>
       <c r="D88" s="134" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E88" s="134"/>
       <c r="F88" s="117"/>
@@ -15366,19 +15365,19 @@
       <c r="K88" s="119"/>
       <c r="L88" s="119"/>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="K89" s="105"/>
       <c r="L89" s="105"/>
     </row>
     <row r="90" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="B90" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F90" s="2"/>
       <c r="K90" s="106"/>
       <c r="L90" s="105"/>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B91" s="64" t="s">
         <v>5</v>
       </c>
@@ -15415,10 +15414,10 @@
         <v>1</v>
       </c>
       <c r="D92" s="92" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E92" s="92" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F92" s="91"/>
       <c r="G92" s="92"/>
@@ -15426,22 +15425,22 @@
       <c r="I92" s="91"/>
       <c r="J92" s="92"/>
       <c r="K92" s="92" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="L92" s="92"/>
     </row>
-    <row r="93" spans="1:12" ht="48" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:12" ht="48" x14ac:dyDescent="0.25">
       <c r="B93" s="91"/>
       <c r="C93" s="111">
         <v>2</v>
       </c>
       <c r="D93" s="92" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E93" s="92"/>
       <c r="F93" s="91"/>
       <c r="G93" s="92" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H93" s="91"/>
       <c r="I93" s="91"/>
@@ -15449,13 +15448,13 @@
       <c r="K93" s="92"/>
       <c r="L93" s="92"/>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B94" s="91"/>
       <c r="C94" s="111">
         <v>3</v>
       </c>
       <c r="D94" s="92" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E94" s="92"/>
       <c r="F94" s="91"/>
@@ -15464,68 +15463,68 @@
       <c r="I94" s="91"/>
       <c r="J94" s="92"/>
       <c r="K94" s="92" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="L94" s="92"/>
     </row>
-    <row r="95" spans="1:12" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:12" ht="71.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B95" s="91"/>
       <c r="C95" s="111">
         <v>4</v>
       </c>
       <c r="D95" s="92" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E95" s="92"/>
       <c r="F95" s="91"/>
       <c r="G95" s="92" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H95" s="91"/>
       <c r="I95" s="91"/>
       <c r="J95" s="92"/>
       <c r="K95" s="92" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="L95" s="92"/>
     </row>
-    <row r="96" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B96" s="91"/>
       <c r="C96" s="111">
         <v>5</v>
       </c>
       <c r="D96" s="92" t="s">
+        <v>167</v>
+      </c>
+      <c r="E96" s="92" t="s">
         <v>168</v>
-      </c>
-      <c r="E96" s="92" t="s">
-        <v>169</v>
       </c>
       <c r="F96" s="91"/>
       <c r="G96" s="93" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H96" s="91"/>
       <c r="I96" s="91"/>
       <c r="J96" s="92"/>
       <c r="K96" s="92" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="L96" s="92"/>
     </row>
-    <row r="97" spans="2:12" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:12" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B97" s="91"/>
       <c r="C97" s="111">
         <v>6</v>
       </c>
       <c r="D97" s="92" t="s">
+        <v>169</v>
+      </c>
+      <c r="E97" s="92" t="s">
         <v>170</v>
-      </c>
-      <c r="E97" s="92" t="s">
-        <v>171</v>
       </c>
       <c r="F97" s="91"/>
       <c r="G97" s="146" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H97" s="91"/>
       <c r="I97" s="91"/>
@@ -15533,13 +15532,13 @@
       <c r="K97" s="92"/>
       <c r="L97" s="92"/>
     </row>
-    <row r="98" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B98" s="91"/>
       <c r="C98" s="111">
         <v>7</v>
       </c>
       <c r="D98" s="92" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E98" s="92"/>
       <c r="F98" s="91"/>
@@ -15550,19 +15549,19 @@
       <c r="K98" s="92"/>
       <c r="L98" s="92"/>
     </row>
-    <row r="99" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="K99" s="105"/>
       <c r="L99" s="105"/>
     </row>
-    <row r="100" spans="2:12" ht="18" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B100" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F100" s="2"/>
       <c r="K100" s="105"/>
       <c r="L100" s="105"/>
     </row>
-    <row r="101" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B101" s="64" t="s">
         <v>5</v>
       </c>
@@ -15593,18 +15592,18 @@
       <c r="K101" s="66"/>
       <c r="L101" s="66"/>
     </row>
-    <row r="102" spans="2:12" ht="24" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:12" ht="24" x14ac:dyDescent="0.25">
       <c r="B102" s="89" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C102" s="57">
         <v>1</v>
       </c>
       <c r="D102" s="89" t="s">
+        <v>99</v>
+      </c>
+      <c r="E102" s="90" t="s">
         <v>100</v>
-      </c>
-      <c r="E102" s="90" t="s">
-        <v>101</v>
       </c>
       <c r="F102" s="89"/>
       <c r="G102" s="90"/>
@@ -15614,18 +15613,18 @@
       <c r="K102" s="107"/>
       <c r="L102" s="107"/>
     </row>
-    <row r="103" spans="2:12" ht="24" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:12" ht="24" x14ac:dyDescent="0.25">
       <c r="B103" s="46" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C103" s="47">
         <v>2</v>
       </c>
       <c r="D103" s="46" t="s">
+        <v>102</v>
+      </c>
+      <c r="E103" s="88" t="s">
         <v>103</v>
-      </c>
-      <c r="E103" s="88" t="s">
-        <v>104</v>
       </c>
       <c r="F103" s="46"/>
       <c r="G103" s="88"/>
@@ -15635,7 +15634,7 @@
       <c r="K103" s="108"/>
       <c r="L103" s="108"/>
     </row>
-    <row r="104" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B104" s="46"/>
       <c r="C104" s="47">
         <v>3</v>
@@ -15650,7 +15649,7 @@
       <c r="K104" s="108"/>
       <c r="L104" s="108"/>
     </row>
-    <row r="105" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B105" s="46"/>
       <c r="C105" s="47">
         <v>4</v>
@@ -15665,15 +15664,15 @@
       <c r="K105" s="108"/>
       <c r="L105" s="108"/>
     </row>
-    <row r="106" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B106" s="44" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C106" s="45">
         <v>5</v>
       </c>
       <c r="D106" s="44" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E106" s="85"/>
       <c r="F106" s="44"/>
@@ -15682,34 +15681,34 @@
       <c r="I106" s="44"/>
       <c r="J106" s="109"/>
       <c r="K106" s="109" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="L106" s="85"/>
     </row>
-    <row r="107" spans="2:12" ht="36" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:12" ht="36" x14ac:dyDescent="0.25">
       <c r="B107" s="44" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C107" s="45">
         <v>6</v>
       </c>
       <c r="D107" s="44" t="s">
+        <v>105</v>
+      </c>
+      <c r="E107" s="85" t="s">
         <v>106</v>
-      </c>
-      <c r="E107" s="85" t="s">
-        <v>107</v>
       </c>
       <c r="F107" s="44"/>
       <c r="G107" s="85"/>
       <c r="H107" s="44"/>
       <c r="I107" s="44"/>
       <c r="J107" s="85" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K107" s="85"/>
       <c r="L107" s="85"/>
     </row>
-    <row r="108" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B108" s="44"/>
       <c r="C108" s="45"/>
       <c r="D108" s="44"/>
@@ -15719,12 +15718,12 @@
       <c r="H108" s="44"/>
       <c r="I108" s="44"/>
       <c r="J108" s="85" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K108" s="85"/>
       <c r="L108" s="85"/>
     </row>
-    <row r="109" spans="2:12" ht="48" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:12" ht="48" x14ac:dyDescent="0.25">
       <c r="B109" s="44"/>
       <c r="C109" s="45"/>
       <c r="D109" s="44"/>
@@ -15734,12 +15733,12 @@
       <c r="H109" s="44"/>
       <c r="I109" s="44"/>
       <c r="J109" s="85" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K109" s="85"/>
       <c r="L109" s="85"/>
     </row>
-    <row r="110" spans="2:12" ht="48" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:12" ht="48" x14ac:dyDescent="0.25">
       <c r="B110" s="44"/>
       <c r="C110" s="45"/>
       <c r="D110" s="44"/>
@@ -15749,20 +15748,20 @@
       <c r="H110" s="44"/>
       <c r="I110" s="44"/>
       <c r="J110" s="85" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K110" s="85"/>
       <c r="L110" s="85"/>
     </row>
-    <row r="111" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B111" s="44" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C111" s="45">
         <v>7</v>
       </c>
       <c r="D111" s="85" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E111" s="85"/>
       <c r="F111" s="44"/>
@@ -15770,18 +15769,18 @@
       <c r="H111" s="44"/>
       <c r="I111" s="44"/>
       <c r="J111" s="85" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K111" s="85"/>
       <c r="L111" s="85"/>
     </row>
-    <row r="112" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B112" s="44"/>
       <c r="C112" s="45">
         <v>8</v>
       </c>
       <c r="D112" s="85" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E112" s="85"/>
       <c r="F112" s="44"/>
@@ -15789,18 +15788,18 @@
       <c r="H112" s="44"/>
       <c r="I112" s="44"/>
       <c r="J112" s="85" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K112" s="85"/>
       <c r="L112" s="85"/>
     </row>
-    <row r="113" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B113" s="44"/>
       <c r="C113" s="45">
         <v>9</v>
       </c>
       <c r="D113" s="85" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E113" s="85"/>
       <c r="F113" s="44"/>
@@ -15808,18 +15807,18 @@
       <c r="H113" s="44"/>
       <c r="I113" s="44"/>
       <c r="J113" s="85" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K113" s="85"/>
       <c r="L113" s="85"/>
     </row>
-    <row r="114" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B114" s="44"/>
       <c r="C114" s="45">
         <v>10</v>
       </c>
       <c r="D114" s="85" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E114" s="85"/>
       <c r="F114" s="44"/>
@@ -15830,13 +15829,13 @@
       <c r="K114" s="85"/>
       <c r="L114" s="85"/>
     </row>
-    <row r="115" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B115" s="44"/>
       <c r="C115" s="45">
         <v>11</v>
       </c>
       <c r="D115" s="85" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E115" s="85"/>
       <c r="F115" s="44"/>
@@ -15847,13 +15846,13 @@
       <c r="K115" s="85"/>
       <c r="L115" s="85"/>
     </row>
-    <row r="116" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B116" s="44"/>
       <c r="C116" s="45">
         <v>12</v>
       </c>
       <c r="D116" s="85" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E116" s="85"/>
       <c r="F116" s="44"/>
@@ -15864,9 +15863,9 @@
       <c r="K116" s="85"/>
       <c r="L116" s="85"/>
     </row>
-    <row r="117" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B117" s="44" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C117" s="45"/>
       <c r="D117" s="85"/>
@@ -15877,13 +15876,13 @@
       <c r="I117" s="44"/>
       <c r="J117" s="85"/>
       <c r="K117" s="85" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="L117" s="85"/>
     </row>
-    <row r="118" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B118" s="44" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C118" s="45"/>
       <c r="D118" s="85"/>
@@ -15896,15 +15895,15 @@
       <c r="K118" s="85"/>
       <c r="L118" s="85"/>
     </row>
-    <row r="119" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B119" s="44" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C119" s="45">
         <v>13</v>
       </c>
       <c r="D119" s="44" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E119" s="86"/>
       <c r="F119" s="44"/>
@@ -15913,17 +15912,17 @@
       <c r="I119" s="44"/>
       <c r="J119" s="85"/>
       <c r="K119" s="109" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="L119" s="85"/>
     </row>
-    <row r="120" spans="2:13" ht="24" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:13" ht="36" x14ac:dyDescent="0.25">
       <c r="B120" s="44"/>
       <c r="C120" s="45">
         <v>14</v>
       </c>
       <c r="D120" s="85" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E120" s="86"/>
       <c r="F120" s="44"/>
@@ -15931,18 +15930,18 @@
       <c r="H120" s="44"/>
       <c r="I120" s="44"/>
       <c r="J120" s="85" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K120" s="85"/>
       <c r="L120" s="85"/>
     </row>
-    <row r="121" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B121" s="44"/>
       <c r="C121" s="45">
         <v>15</v>
       </c>
       <c r="D121" s="85" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E121" s="86"/>
       <c r="F121" s="44"/>
@@ -15950,18 +15949,18 @@
       <c r="H121" s="44"/>
       <c r="I121" s="44"/>
       <c r="J121" s="85" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K121" s="85"/>
       <c r="L121" s="85"/>
     </row>
-    <row r="122" spans="2:13" ht="48" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:13" ht="48" x14ac:dyDescent="0.25">
       <c r="B122" s="44"/>
       <c r="C122" s="45">
         <v>16</v>
       </c>
       <c r="D122" s="85" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E122" s="86"/>
       <c r="F122" s="44"/>
@@ -15969,18 +15968,18 @@
       <c r="H122" s="44"/>
       <c r="I122" s="44"/>
       <c r="J122" s="85" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K122" s="85"/>
       <c r="L122" s="85"/>
     </row>
-    <row r="123" spans="2:13" ht="48" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:13" ht="48" x14ac:dyDescent="0.25">
       <c r="B123" s="44"/>
       <c r="C123" s="45">
         <v>17</v>
       </c>
       <c r="D123" s="85" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E123" s="86"/>
       <c r="F123" s="44"/>
@@ -15988,18 +15987,18 @@
       <c r="H123" s="44"/>
       <c r="I123" s="44"/>
       <c r="J123" s="85" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K123" s="85"/>
       <c r="L123" s="85"/>
     </row>
-    <row r="124" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B124" s="44"/>
       <c r="C124" s="45">
         <v>18</v>
       </c>
       <c r="D124" s="85" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E124" s="85"/>
       <c r="F124" s="44"/>
@@ -16011,13 +16010,13 @@
       <c r="L124" s="85"/>
       <c r="M124" s="106"/>
     </row>
-    <row r="125" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B125" s="44"/>
       <c r="C125" s="45">
         <v>19</v>
       </c>
       <c r="D125" s="85" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E125" s="87"/>
       <c r="F125" s="44"/>
@@ -16028,57 +16027,57 @@
       <c r="K125" s="85"/>
       <c r="L125" s="85"/>
     </row>
-    <row r="126" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B126" s="43" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C126" s="25">
         <v>20</v>
       </c>
       <c r="D126" s="43" t="s">
+        <v>156</v>
+      </c>
+      <c r="E126" s="43" t="s">
         <v>157</v>
-      </c>
-      <c r="E126" s="43" t="s">
-        <v>158</v>
       </c>
       <c r="F126" s="43"/>
       <c r="G126" s="79"/>
       <c r="H126" s="43"/>
       <c r="I126" s="43"/>
       <c r="J126" s="43" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K126" s="72"/>
       <c r="L126" s="72"/>
     </row>
-    <row r="127" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B127" s="43"/>
       <c r="C127" s="25">
         <v>21</v>
       </c>
       <c r="D127" s="43" t="s">
+        <v>158</v>
+      </c>
+      <c r="E127" s="43" t="s">
         <v>159</v>
-      </c>
-      <c r="E127" s="43" t="s">
-        <v>160</v>
       </c>
       <c r="F127" s="43"/>
       <c r="G127" s="79"/>
       <c r="H127" s="43"/>
       <c r="I127" s="43"/>
       <c r="J127" s="43" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K127" s="72"/>
       <c r="L127" s="72"/>
     </row>
-    <row r="128" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B128" s="43"/>
       <c r="C128" s="25">
         <v>22</v>
       </c>
       <c r="D128" s="43" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E128" s="43"/>
       <c r="F128" s="43"/>
@@ -16087,11 +16086,11 @@
       <c r="I128" s="43"/>
       <c r="J128" s="43"/>
       <c r="K128" s="72" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="L128" s="72"/>
     </row>
-    <row r="129" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B129" s="43"/>
       <c r="C129" s="25"/>
       <c r="D129" s="43"/>
@@ -16104,15 +16103,15 @@
       <c r="K129" s="72"/>
       <c r="L129" s="72"/>
     </row>
-    <row r="130" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B130" s="71" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C130" s="25">
         <v>23</v>
       </c>
       <c r="D130" s="43" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E130" s="43"/>
       <c r="F130" s="43"/>
@@ -16121,17 +16120,17 @@
       <c r="I130" s="43"/>
       <c r="J130" s="79"/>
       <c r="K130" s="79" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L130" s="72"/>
     </row>
-    <row r="131" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B131" s="71"/>
       <c r="C131" s="25">
         <v>24</v>
       </c>
       <c r="D131" s="71" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E131" s="71"/>
       <c r="F131" s="71"/>
@@ -16142,13 +16141,13 @@
       <c r="K131" s="72"/>
       <c r="L131" s="72"/>
     </row>
-    <row r="132" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B132" s="71"/>
       <c r="C132" s="25">
         <v>25</v>
       </c>
       <c r="D132" s="71" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E132" s="71"/>
       <c r="F132" s="71"/>
@@ -16159,18 +16158,18 @@
       <c r="K132" s="72"/>
       <c r="L132" s="72"/>
     </row>
-    <row r="133" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="D133" s="100"/>
       <c r="K133" s="103"/>
       <c r="L133" s="106"/>
     </row>
-    <row r="134" spans="2:12" ht="18" x14ac:dyDescent="0.35">
+    <row r="134" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B134" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F134" s="2"/>
     </row>
-    <row r="135" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B135" s="64" t="s">
         <v>5</v>
       </c>
@@ -16201,11 +16200,11 @@
       <c r="K135" s="66"/>
       <c r="L135" s="66"/>
     </row>
-    <row r="136" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B136" s="82"/>
       <c r="C136" s="35"/>
       <c r="D136" s="82" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E136" s="82" t="s">
         <v>87</v>
@@ -16215,18 +16214,18 @@
       <c r="H136" s="82"/>
       <c r="I136" s="82"/>
       <c r="J136" s="83" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="K136" s="83" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L136" s="83"/>
     </row>
-    <row r="137" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B137" s="82"/>
       <c r="C137" s="35"/>
       <c r="D137" s="82" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E137" s="82"/>
       <c r="F137" s="82"/>
@@ -16235,18 +16234,18 @@
       <c r="I137" s="82"/>
       <c r="J137" s="83"/>
       <c r="K137" s="83" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="L137" s="83"/>
     </row>
-    <row r="138" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B138" s="82"/>
       <c r="C138" s="35"/>
       <c r="D138" s="82" t="s">
+        <v>146</v>
+      </c>
+      <c r="E138" s="82" t="s">
         <v>147</v>
-      </c>
-      <c r="E138" s="82" t="s">
-        <v>148</v>
       </c>
       <c r="F138" s="82"/>
       <c r="G138" s="83"/>
@@ -16256,14 +16255,14 @@
       <c r="K138" s="83"/>
       <c r="L138" s="83"/>
     </row>
-    <row r="139" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B139" s="82"/>
       <c r="C139" s="35"/>
       <c r="D139" s="82" t="s">
+        <v>148</v>
+      </c>
+      <c r="E139" s="82" t="s">
         <v>149</v>
-      </c>
-      <c r="E139" s="82" t="s">
-        <v>150</v>
       </c>
       <c r="F139" s="82"/>
       <c r="G139" s="83"/>
@@ -16273,16 +16272,16 @@
       <c r="K139" s="83"/>
       <c r="L139" s="83"/>
     </row>
-    <row r="140" spans="2:12" ht="24.6" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:12" ht="36.75" x14ac:dyDescent="0.25">
       <c r="B140" s="82"/>
       <c r="C140" s="35"/>
       <c r="D140" s="82" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E140" s="82"/>
       <c r="F140" s="82"/>
       <c r="G140" s="84" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H140" s="82"/>
       <c r="I140" s="82"/>
@@ -16290,11 +16289,11 @@
       <c r="K140" s="83"/>
       <c r="L140" s="83"/>
     </row>
-    <row r="141" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B141" s="82"/>
       <c r="C141" s="35"/>
       <c r="D141" s="82" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E141" s="82"/>
       <c r="F141" s="82"/>
@@ -16303,17 +16302,17 @@
       <c r="I141" s="82"/>
       <c r="J141" s="83"/>
       <c r="K141" s="83" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L141" s="83"/>
     </row>
-    <row r="143" spans="2:12" ht="18" x14ac:dyDescent="0.35">
+    <row r="143" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B143" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F143" s="2"/>
     </row>
-    <row r="144" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B144" s="64" t="s">
         <v>5</v>
       </c>
@@ -16344,7 +16343,7 @@
       <c r="K144" s="66"/>
       <c r="L144" s="66"/>
     </row>
-    <row r="145" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B145" s="43"/>
       <c r="C145" s="25"/>
       <c r="D145" s="43"/>
@@ -16357,7 +16356,7 @@
       <c r="K145" s="79"/>
       <c r="L145" s="79"/>
     </row>
-    <row r="146" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B146" s="43"/>
       <c r="C146" s="25"/>
       <c r="D146" s="43"/>
@@ -16370,7 +16369,7 @@
       <c r="K146" s="79"/>
       <c r="L146" s="79"/>
     </row>
-    <row r="147" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B147" s="43"/>
       <c r="C147" s="25"/>
       <c r="D147" s="43"/>
@@ -16383,19 +16382,19 @@
       <c r="K147" s="79"/>
       <c r="L147" s="79"/>
     </row>
-    <row r="148" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="K148" s="105"/>
       <c r="L148" s="105"/>
     </row>
     <row r="149" spans="2:12" ht="18" x14ac:dyDescent="0.35">
       <c r="B149" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F149" s="2"/>
       <c r="K149" s="106"/>
       <c r="L149" s="105"/>
     </row>
-    <row r="150" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B150" s="69" t="s">
         <v>5</v>
       </c>
@@ -16426,9 +16425,9 @@
       <c r="K150" s="70"/>
       <c r="L150" s="70"/>
     </row>
-    <row r="151" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="151" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B151" s="73" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C151" s="113"/>
       <c r="D151" s="73" t="s">
@@ -16443,15 +16442,15 @@
       </c>
       <c r="J151" s="74"/>
       <c r="K151" s="74" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L151" s="74"/>
     </row>
-    <row r="152" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="152" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B152" s="73"/>
       <c r="C152" s="113"/>
       <c r="D152" s="73" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E152" s="73" t="s">
         <v>31</v>
@@ -16464,14 +16463,14 @@
       <c r="K152" s="74"/>
       <c r="L152" s="74"/>
     </row>
-    <row r="153" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B153" s="73"/>
       <c r="C153" s="113"/>
       <c r="D153" s="73" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E153" s="73" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F153" s="73"/>
       <c r="G153" s="74"/>
@@ -16481,11 +16480,11 @@
       <c r="K153" s="74"/>
       <c r="L153" s="74"/>
     </row>
-    <row r="154" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="154" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B154" s="73"/>
       <c r="C154" s="113"/>
       <c r="D154" s="73" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E154" s="75"/>
       <c r="F154" s="73"/>
@@ -16496,11 +16495,11 @@
       <c r="K154" s="74"/>
       <c r="L154" s="74"/>
     </row>
-    <row r="155" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="155" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B155" s="73"/>
       <c r="C155" s="113"/>
       <c r="D155" s="76" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E155" s="76"/>
       <c r="F155" s="73"/>
@@ -16511,11 +16510,11 @@
       <c r="K155" s="74"/>
       <c r="L155" s="74"/>
     </row>
-    <row r="156" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="156" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B156" s="73"/>
       <c r="C156" s="113"/>
       <c r="D156" s="76" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E156" s="76"/>
       <c r="F156" s="73"/>
@@ -16524,19 +16523,19 @@
       <c r="I156" s="73"/>
       <c r="J156" s="74"/>
       <c r="K156" s="74" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="L156" s="74"/>
     </row>
-    <row r="157" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="157" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B157" s="73"/>
       <c r="C157" s="113"/>
       <c r="D157" s="73" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E157" s="75"/>
       <c r="F157" s="73" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G157" s="74"/>
       <c r="H157" s="73"/>
@@ -16545,11 +16544,11 @@
       <c r="K157" s="74"/>
       <c r="L157" s="74"/>
     </row>
-    <row r="158" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="158" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B158" s="73"/>
       <c r="C158" s="113"/>
       <c r="D158" s="73" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E158" s="73"/>
       <c r="F158" s="73"/>
@@ -16560,11 +16559,11 @@
       <c r="K158" s="74"/>
       <c r="L158" s="74"/>
     </row>
-    <row r="159" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="159" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B159" s="73"/>
       <c r="C159" s="113"/>
       <c r="D159" s="73" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E159" s="73"/>
       <c r="F159" s="73"/>
@@ -16575,11 +16574,11 @@
       <c r="K159" s="74"/>
       <c r="L159" s="74"/>
     </row>
-    <row r="160" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="160" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B160" s="73"/>
       <c r="C160" s="113"/>
       <c r="D160" s="73" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E160" s="77"/>
       <c r="F160" s="73"/>
@@ -16590,11 +16589,11 @@
       <c r="K160" s="74"/>
       <c r="L160" s="74"/>
     </row>
-    <row r="161" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="161" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B161" s="73"/>
       <c r="C161" s="113"/>
       <c r="D161" s="73" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E161" s="73"/>
       <c r="F161" s="73"/>
@@ -16605,28 +16604,28 @@
       <c r="K161" s="74"/>
       <c r="L161" s="74"/>
     </row>
-    <row r="162" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="162" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B162" s="73"/>
       <c r="C162" s="113"/>
       <c r="D162" s="73" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E162" s="78"/>
       <c r="F162" s="73"/>
       <c r="G162" s="74"/>
       <c r="H162" s="73"/>
       <c r="I162" s="73"/>
-      <c r="J162" s="154" t="s">
-        <v>308</v>
+      <c r="J162" s="147" t="s">
+        <v>307</v>
       </c>
       <c r="K162" s="74"/>
       <c r="L162" s="74"/>
     </row>
-    <row r="163" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="163" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B163" s="73"/>
       <c r="C163" s="113"/>
       <c r="D163" s="73" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E163" s="73"/>
       <c r="F163" s="73"/>
@@ -16635,15 +16634,15 @@
       <c r="I163" s="73"/>
       <c r="J163" s="74"/>
       <c r="K163" s="74" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="L163" s="74"/>
     </row>
-    <row r="164" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="164" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B164" s="73"/>
       <c r="C164" s="113"/>
       <c r="D164" s="74" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E164" s="78"/>
       <c r="F164" s="73"/>
@@ -16654,14 +16653,14 @@
       <c r="K164" s="74"/>
       <c r="L164" s="74"/>
     </row>
-    <row r="165" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="165" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B165" s="73"/>
       <c r="C165" s="113"/>
       <c r="D165" s="73" t="s">
+        <v>181</v>
+      </c>
+      <c r="E165" s="73" t="s">
         <v>182</v>
-      </c>
-      <c r="E165" s="73" t="s">
-        <v>183</v>
       </c>
       <c r="F165" s="73"/>
       <c r="G165" s="74"/>
@@ -16671,30 +16670,30 @@
       <c r="K165" s="74"/>
       <c r="L165" s="74"/>
     </row>
-    <row r="166" spans="2:12" ht="60.6" x14ac:dyDescent="0.3">
+    <row r="166" spans="2:12" ht="60.75" x14ac:dyDescent="0.25">
       <c r="B166" s="73"/>
       <c r="C166" s="113"/>
       <c r="D166" s="73" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E166" s="73"/>
       <c r="F166" s="73"/>
       <c r="G166" s="74" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H166" s="73"/>
       <c r="I166" s="73"/>
       <c r="J166" s="74"/>
       <c r="K166" s="74" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="L166" s="74"/>
     </row>
-    <row r="167" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="167" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B167" s="73"/>
       <c r="C167" s="113"/>
       <c r="D167" s="73" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E167" s="73"/>
       <c r="F167" s="73"/>
@@ -16705,51 +16704,51 @@
       <c r="K167" s="74"/>
       <c r="L167" s="74"/>
     </row>
-    <row r="170" spans="2:12" ht="34.799999999999997" x14ac:dyDescent="0.3">
+    <row r="170" spans="2:12" ht="34.9" x14ac:dyDescent="0.3">
       <c r="B170" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E170" s="2"/>
       <c r="F170" s="2"/>
     </row>
-    <row r="171" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B171" s="147" t="s">
+    <row r="171" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B171" s="148" t="s">
         <v>0</v>
       </c>
-      <c r="C171" s="149" t="s">
+      <c r="C171" s="150" t="s">
         <v>14</v>
       </c>
-      <c r="D171" s="149"/>
-      <c r="E171" s="149"/>
-      <c r="F171" s="149"/>
-      <c r="G171" s="149"/>
-      <c r="H171" s="149"/>
-    </row>
-    <row r="172" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B172" s="148"/>
-      <c r="C172" s="149" t="s">
-        <v>265</v>
-      </c>
-      <c r="D172" s="149"/>
-      <c r="E172" s="149"/>
-      <c r="F172" s="149"/>
-      <c r="G172" s="149"/>
-      <c r="H172" s="149"/>
-    </row>
-    <row r="173" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="D171" s="150"/>
+      <c r="E171" s="150"/>
+      <c r="F171" s="150"/>
+      <c r="G171" s="150"/>
+      <c r="H171" s="150"/>
+    </row>
+    <row r="172" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B172" s="149"/>
+      <c r="C172" s="150" t="s">
+        <v>264</v>
+      </c>
+      <c r="D172" s="150"/>
+      <c r="E172" s="150"/>
+      <c r="F172" s="150"/>
+      <c r="G172" s="150"/>
+      <c r="H172" s="150"/>
+    </row>
+    <row r="173" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B173" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C173" s="150" t="s">
-        <v>264</v>
-      </c>
-      <c r="D173" s="150"/>
-      <c r="E173" s="150"/>
-      <c r="F173" s="150"/>
-      <c r="G173" s="150"/>
-      <c r="H173" s="150"/>
-    </row>
-    <row r="174" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C173" s="151" t="s">
+        <v>263</v>
+      </c>
+      <c r="D173" s="151"/>
+      <c r="E173" s="151"/>
+      <c r="F173" s="151"/>
+      <c r="G173" s="151"/>
+      <c r="H173" s="151"/>
+    </row>
+    <row r="174" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B174" s="5"/>
       <c r="C174" s="12"/>
       <c r="D174" s="17"/>
@@ -16758,9 +16757,9 @@
       <c r="G174" s="61"/>
       <c r="H174" s="5"/>
     </row>
-    <row r="175" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="175" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B175" s="120" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C175" s="103"/>
       <c r="F175" s="9"/>
@@ -16769,62 +16768,62 @@
       <c r="B176" s="120"/>
       <c r="C176" s="103"/>
     </row>
-    <row r="177" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="177" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B177" s="121" t="s">
+        <v>266</v>
+      </c>
+      <c r="C177" s="121" t="s">
+        <v>279</v>
+      </c>
+      <c r="D177" s="121" t="s">
         <v>267</v>
-      </c>
-      <c r="C177" s="121" t="s">
-        <v>280</v>
-      </c>
-      <c r="D177" s="121" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="178" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B178" s="122" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C178" s="127" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D178" s="80" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="179" spans="2:12" ht="24" x14ac:dyDescent="0.3">
       <c r="B179" s="123" t="s">
+        <v>269</v>
+      </c>
+      <c r="C179" s="128" t="s">
+        <v>276</v>
+      </c>
+      <c r="D179" s="90" t="s">
         <v>270</v>
       </c>
-      <c r="C179" s="128" t="s">
+    </row>
+    <row r="180" spans="2:12" ht="108" x14ac:dyDescent="0.25">
+      <c r="B180" s="124" t="s">
+        <v>271</v>
+      </c>
+      <c r="C180" s="129" t="s">
         <v>277</v>
       </c>
-      <c r="D179" s="90" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="180" spans="2:12" ht="108" x14ac:dyDescent="0.3">
-      <c r="B180" s="124" t="s">
+      <c r="D180" s="83" t="s">
         <v>272</v>
       </c>
-      <c r="C180" s="129" t="s">
+    </row>
+    <row r="181" spans="2:12" ht="48" x14ac:dyDescent="0.25">
+      <c r="B181" s="125" t="s">
+        <v>273</v>
+      </c>
+      <c r="C181" s="130" t="s">
         <v>278</v>
       </c>
-      <c r="D180" s="83" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="181" spans="2:12" ht="48" x14ac:dyDescent="0.3">
-      <c r="B181" s="125" t="s">
+      <c r="D181" s="126" t="s">
         <v>274</v>
       </c>
-      <c r="C181" s="130" t="s">
-        <v>279</v>
-      </c>
-      <c r="D181" s="126" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="189" spans="2:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="189" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B189" s="6" t="s">
         <v>2</v>
       </c>
@@ -16835,15 +16834,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="191" spans="2:12" ht="18" x14ac:dyDescent="0.35">
+    <row r="191" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B191" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F191" s="2"/>
       <c r="K191" s="106"/>
       <c r="L191" s="105"/>
     </row>
-    <row r="192" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="192" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B192" s="69" t="s">
         <v>5</v>
       </c>
@@ -16874,7 +16873,7 @@
       <c r="K192" s="70"/>
       <c r="L192" s="70"/>
     </row>
-    <row r="193" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="193" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B193" s="11" t="s">
         <v>29</v>
       </c>
@@ -16889,7 +16888,7 @@
       <c r="K193" s="11"/>
       <c r="L193" s="11"/>
     </row>
-    <row r="194" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="194" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B194" s="11"/>
       <c r="C194" s="15"/>
       <c r="D194" s="18"/>
@@ -16902,7 +16901,7 @@
       <c r="K194" s="11"/>
       <c r="L194" s="11"/>
     </row>
-    <row r="195" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="195" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B195" s="11"/>
       <c r="C195" s="15"/>
       <c r="D195" s="18"/>
@@ -16994,11 +16993,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -17016,11 +17015,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -17038,11 +17037,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -17060,11 +17059,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -17082,11 +17081,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -17104,11 +17103,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -17126,11 +17125,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -17148,11 +17147,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -17170,11 +17169,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -17192,11 +17191,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -17214,11 +17213,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -17236,11 +17235,11 @@
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -17258,11 +17257,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -17280,11 +17279,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -17302,11 +17301,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -17324,11 +17323,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -17346,11 +17345,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -17368,11 +17367,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -17390,11 +17389,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -17412,11 +17411,11 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -17434,11 +17433,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -17456,11 +17455,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -17478,11 +17477,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -17500,11 +17499,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -17522,11 +17521,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -17544,11 +17543,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -17566,11 +17565,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -17588,11 +17587,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -17610,11 +17609,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -17632,11 +17631,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -17654,11 +17653,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -17676,11 +17675,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -17698,11 +17697,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -17720,11 +17719,11 @@
   <sheetViews>
     <sheetView zoomScale="86" zoomScaleNormal="86" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -17742,11 +17741,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -17764,11 +17763,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -17786,11 +17785,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -17808,16 +17807,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -17836,11 +17835,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -17858,11 +17857,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -17880,11 +17879,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -17902,11 +17901,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -17924,11 +17923,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -17946,11 +17945,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -17968,11 +17967,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -17990,11 +17989,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -18012,11 +18011,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>

</xml_diff>